<commit_message>
Lots of new documents
</commit_message>
<xml_diff>
--- a/Documentation/SCRUM_Backlogs_Template-1.xlsx
+++ b/Documentation/SCRUM_Backlogs_Template-1.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25629"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9954B842-44EF-4A8E-A069-33781852116D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="975" yWindow="0" windowWidth="24195" windowHeight="7680"/>
+    <workbookView xWindow="5892" yWindow="3120" windowWidth="15372" windowHeight="8280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
     <sheet name="Sprint 1" sheetId="2" r:id="rId2"/>
     <sheet name="Sprint x (copy template!)" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211" concurrentCalc="0"/>
+  <calcPr calcId="122211"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -134,7 +135,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -328,11 +329,26 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -342,20 +358,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -363,6 +370,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -372,18 +382,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -684,24 +685,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="74.140625" style="8" customWidth="1"/>
+    <col min="1" max="1" width="5.33203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="74.109375" style="8" customWidth="1"/>
     <col min="3" max="3" width="12" style="2" customWidth="1"/>
-    <col min="4" max="5" width="11.28515625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="2"/>
-    <col min="7" max="7" width="49.7109375" style="8" customWidth="1"/>
+    <col min="4" max="5" width="11.33203125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" style="2"/>
+    <col min="7" max="7" width="49.6640625" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -722,7 +723,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="21"/>
       <c r="B2" s="20"/>
       <c r="C2" s="21"/>
@@ -735,7 +736,7 @@
       <c r="F2" s="21"/>
       <c r="G2" s="20"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -752,7 +753,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -769,7 +770,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -777,7 +778,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -785,7 +786,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B29" s="8" t="s">
         <v>35</v>
       </c>
@@ -804,35 +805,35 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" customWidth="1"/>
-    <col min="2" max="2" width="50.28515625" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" style="10" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" style="10" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" style="10" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" style="10" customWidth="1"/>
-    <col min="7" max="7" width="29.42578125" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" customWidth="1"/>
+    <col min="2" max="2" width="50.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" style="10" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" style="10" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" style="10" customWidth="1"/>
+    <col min="6" max="6" width="17.44140625" style="10" customWidth="1"/>
+    <col min="7" max="7" width="29.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="6"/>
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
@@ -840,7 +841,7 @@
         <v>43412</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
@@ -848,7 +849,7 @@
         <v>43432</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>10</v>
       </c>
@@ -856,57 +857,57 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B8" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="29" t="s">
+      <c r="C8" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="31"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="28"/>
       <c r="G8" s="18" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9">
         <v>1</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="26"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="31"/>
       <c r="G9" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="26"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="31"/>
       <c r="G10" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="13"/>
@@ -917,57 +918,57 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="26"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="31"/>
       <c r="G12" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="27" t="s">
+    <row r="15" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="27" t="s">
+      <c r="B15" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="22" t="s">
+      <c r="C15" s="24" t="s">
         <v>21</v>
       </c>
       <c r="D15" s="20" t="s">
         <v>24</v>
       </c>
       <c r="E15" s="20"/>
-      <c r="F15" s="22" t="s">
+      <c r="F15" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="G15" s="22" t="s">
+      <c r="G15" s="24" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="28"/>
-      <c r="B16" s="28"/>
-      <c r="C16" s="23"/>
+    <row r="16" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="23"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="25"/>
       <c r="D16" s="19" t="s">
         <v>17</v>
       </c>
       <c r="E16" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>1</v>
       </c>
@@ -990,7 +991,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>2</v>
       </c>
@@ -1011,7 +1012,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>3</v>
       </c>
@@ -1030,7 +1031,7 @@
       </c>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="2"/>
       <c r="C20" s="11"/>
@@ -1039,7 +1040,7 @@
       <c r="F20" s="11"/>
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" s="2"/>
       <c r="C21" s="11"/>
@@ -1048,7 +1049,7 @@
       <c r="F21" s="11"/>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="B22" s="2"/>
       <c r="C22" s="11"/>
@@ -1057,7 +1058,7 @@
       <c r="F22" s="11"/>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
       <c r="B23" s="2"/>
       <c r="C23" s="11"/>
@@ -1066,7 +1067,7 @@
       <c r="F23" s="11"/>
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
       <c r="B24" s="2"/>
       <c r="C24" s="11"/>
@@ -1075,7 +1076,7 @@
       <c r="F24" s="11"/>
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" s="2"/>
       <c r="C25" s="11"/>
@@ -1084,7 +1085,7 @@
       <c r="F25" s="11"/>
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
       <c r="B26" s="2"/>
       <c r="C26" s="11"/>
@@ -1093,7 +1094,7 @@
       <c r="F26" s="11"/>
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" s="2"/>
       <c r="C27" s="11"/>
@@ -1102,7 +1103,7 @@
       <c r="F27" s="11"/>
       <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
       <c r="B28" s="2"/>
       <c r="C28" s="11"/>
@@ -1111,7 +1112,7 @@
       <c r="F28" s="11"/>
       <c r="G28" s="2"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
       <c r="B29" s="2"/>
       <c r="C29" s="11"/>
@@ -1120,7 +1121,7 @@
       <c r="F29" s="11"/>
       <c r="G29" s="2"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
       <c r="B30" s="2"/>
       <c r="C30" s="11"/>
@@ -1129,7 +1130,7 @@
       <c r="F30" s="11"/>
       <c r="G30" s="2"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="3"/>
       <c r="B31" s="2"/>
       <c r="C31" s="11"/>
@@ -1138,7 +1139,7 @@
       <c r="F31" s="11"/>
       <c r="G31" s="2"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="3"/>
       <c r="B32" s="2"/>
       <c r="C32" s="11"/>
@@ -1147,7 +1148,7 @@
       <c r="F32" s="11"/>
       <c r="G32" s="2"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="3"/>
       <c r="B33" s="2"/>
       <c r="C33" s="11"/>
@@ -1156,7 +1157,7 @@
       <c r="F33" s="11"/>
       <c r="G33" s="2"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="3"/>
       <c r="B34" s="2"/>
       <c r="C34" s="11"/>
@@ -1165,7 +1166,7 @@
       <c r="F34" s="11"/>
       <c r="G34" s="2"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="3"/>
       <c r="B35" s="2"/>
       <c r="C35" s="11"/>
@@ -1174,7 +1175,7 @@
       <c r="F35" s="11"/>
       <c r="G35" s="2"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="3"/>
       <c r="B36" s="2"/>
       <c r="C36" s="11"/>
@@ -1183,7 +1184,7 @@
       <c r="F36" s="11"/>
       <c r="G36" s="2"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="3"/>
       <c r="B37" s="2"/>
       <c r="C37" s="11"/>
@@ -1192,7 +1193,7 @@
       <c r="F37" s="11"/>
       <c r="G37" s="2"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="3"/>
       <c r="B38" s="2"/>
       <c r="C38" s="11"/>
@@ -1201,7 +1202,7 @@
       <c r="F38" s="11"/>
       <c r="G38" s="2"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="3"/>
       <c r="B39" s="2"/>
       <c r="C39" s="11"/>
@@ -1210,7 +1211,7 @@
       <c r="F39" s="11"/>
       <c r="G39" s="2"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="3"/>
       <c r="B40" s="2"/>
       <c r="C40" s="11"/>
@@ -1219,7 +1220,7 @@
       <c r="F40" s="11"/>
       <c r="G40" s="2"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="3"/>
       <c r="B41" s="2"/>
       <c r="C41" s="11"/>
@@ -1228,7 +1229,7 @@
       <c r="F41" s="11"/>
       <c r="G41" s="2"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="3"/>
       <c r="B42" s="2"/>
       <c r="C42" s="11"/>
@@ -1237,7 +1238,7 @@
       <c r="F42" s="11"/>
       <c r="G42" s="2"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="3"/>
       <c r="B43" s="2"/>
       <c r="C43" s="11"/>
@@ -1246,7 +1247,7 @@
       <c r="F43" s="11"/>
       <c r="G43" s="2"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="3"/>
       <c r="B44" s="2"/>
       <c r="C44" s="11"/>
@@ -1257,16 +1258,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="D15:E15"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="C15:C16"/>
     <mergeCell ref="F15:F16"/>
     <mergeCell ref="C8:F8"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="D15:E15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -1274,47 +1275,47 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" customWidth="1"/>
-    <col min="2" max="2" width="50.28515625" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" style="10" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" style="10" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" style="10" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" style="10" customWidth="1"/>
-    <col min="7" max="7" width="29.42578125" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" customWidth="1"/>
+    <col min="2" max="2" width="50.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" style="10" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" style="10" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" style="10" customWidth="1"/>
+    <col min="6" max="6" width="17.44140625" style="10" customWidth="1"/>
+    <col min="7" max="7" width="29.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="6"/>
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="7"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="7"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>10</v>
       </c>
@@ -1322,47 +1323,47 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
         <v>0</v>
       </c>
       <c r="B8" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="34" t="s">
+      <c r="C8" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="36"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="39"/>
       <c r="G8" s="15" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9"/>
       <c r="B9" s="8"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="26"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="31"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="26"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="31"/>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="13"/>
@@ -1371,55 +1372,55 @@
       <c r="F11" s="12"/>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="26"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="31"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="37" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="37" t="s">
+      <c r="B15" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="32" t="s">
+      <c r="C15" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="39" t="s">
+      <c r="D15" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="E15" s="39"/>
-      <c r="F15" s="32" t="s">
+      <c r="E15" s="36"/>
+      <c r="F15" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="G15" s="32" t="s">
+      <c r="G15" s="34" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="38"/>
-      <c r="B16" s="38"/>
-      <c r="C16" s="33"/>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="33"/>
+      <c r="B16" s="33"/>
+      <c r="C16" s="35"/>
       <c r="D16" s="16" t="s">
         <v>17</v>
       </c>
       <c r="E16" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="F16" s="33"/>
-      <c r="G16" s="33"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F16" s="35"/>
+      <c r="G16" s="35"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="2"/>
       <c r="C17" s="11"/>
@@ -1428,7 +1429,7 @@
       <c r="F17" s="11"/>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="2"/>
       <c r="C18" s="11"/>
@@ -1437,7 +1438,7 @@
       <c r="F18" s="11"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="2"/>
       <c r="C19" s="11"/>
@@ -1446,7 +1447,7 @@
       <c r="F19" s="11"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="2"/>
       <c r="C20" s="11"/>
@@ -1455,7 +1456,7 @@
       <c r="F20" s="11"/>
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" s="2"/>
       <c r="C21" s="11"/>
@@ -1464,7 +1465,7 @@
       <c r="F21" s="11"/>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="B22" s="2"/>
       <c r="C22" s="11"/>
@@ -1473,7 +1474,7 @@
       <c r="F22" s="11"/>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
       <c r="B23" s="2"/>
       <c r="C23" s="11"/>
@@ -1482,7 +1483,7 @@
       <c r="F23" s="11"/>
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
       <c r="B24" s="2"/>
       <c r="C24" s="11"/>
@@ -1491,7 +1492,7 @@
       <c r="F24" s="11"/>
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" s="2"/>
       <c r="C25" s="11"/>
@@ -1500,7 +1501,7 @@
       <c r="F25" s="11"/>
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
       <c r="B26" s="2"/>
       <c r="C26" s="11"/>
@@ -1509,7 +1510,7 @@
       <c r="F26" s="11"/>
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" s="2"/>
       <c r="C27" s="11"/>
@@ -1518,7 +1519,7 @@
       <c r="F27" s="11"/>
       <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
       <c r="B28" s="2"/>
       <c r="C28" s="11"/>
@@ -1527,7 +1528,7 @@
       <c r="F28" s="11"/>
       <c r="G28" s="2"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
       <c r="B29" s="2"/>
       <c r="C29" s="11"/>
@@ -1536,7 +1537,7 @@
       <c r="F29" s="11"/>
       <c r="G29" s="2"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
       <c r="B30" s="2"/>
       <c r="C30" s="11"/>
@@ -1545,7 +1546,7 @@
       <c r="F30" s="11"/>
       <c r="G30" s="2"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="3"/>
       <c r="B31" s="2"/>
       <c r="C31" s="11"/>
@@ -1554,7 +1555,7 @@
       <c r="F31" s="11"/>
       <c r="G31" s="2"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="3"/>
       <c r="B32" s="2"/>
       <c r="C32" s="11"/>
@@ -1563,7 +1564,7 @@
       <c r="F32" s="11"/>
       <c r="G32" s="2"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="3"/>
       <c r="B33" s="2"/>
       <c r="C33" s="11"/>
@@ -1572,7 +1573,7 @@
       <c r="F33" s="11"/>
       <c r="G33" s="2"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="3"/>
       <c r="B34" s="2"/>
       <c r="C34" s="11"/>
@@ -1581,7 +1582,7 @@
       <c r="F34" s="11"/>
       <c r="G34" s="2"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="3"/>
       <c r="B35" s="2"/>
       <c r="C35" s="11"/>
@@ -1590,7 +1591,7 @@
       <c r="F35" s="11"/>
       <c r="G35" s="2"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="3"/>
       <c r="B36" s="2"/>
       <c r="C36" s="11"/>
@@ -1599,7 +1600,7 @@
       <c r="F36" s="11"/>
       <c r="G36" s="2"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="3"/>
       <c r="B37" s="2"/>
       <c r="C37" s="11"/>
@@ -1608,7 +1609,7 @@
       <c r="F37" s="11"/>
       <c r="G37" s="2"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="3"/>
       <c r="B38" s="2"/>
       <c r="C38" s="11"/>
@@ -1617,7 +1618,7 @@
       <c r="F38" s="11"/>
       <c r="G38" s="2"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="3"/>
       <c r="B39" s="2"/>
       <c r="C39" s="11"/>
@@ -1626,7 +1627,7 @@
       <c r="F39" s="11"/>
       <c r="G39" s="2"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="3"/>
       <c r="B40" s="2"/>
       <c r="C40" s="11"/>
@@ -1635,7 +1636,7 @@
       <c r="F40" s="11"/>
       <c r="G40" s="2"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="3"/>
       <c r="B41" s="2"/>
       <c r="C41" s="11"/>
@@ -1644,7 +1645,7 @@
       <c r="F41" s="11"/>
       <c r="G41" s="2"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="3"/>
       <c r="B42" s="2"/>
       <c r="C42" s="11"/>
@@ -1653,7 +1654,7 @@
       <c r="F42" s="11"/>
       <c r="G42" s="2"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="3"/>
       <c r="B43" s="2"/>
       <c r="C43" s="11"/>
@@ -1662,7 +1663,7 @@
       <c r="F43" s="11"/>
       <c r="G43" s="2"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="3"/>
       <c r="B44" s="2"/>
       <c r="C44" s="11"/>
@@ -1673,16 +1674,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="C12:F12"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="C15:C16"/>
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="F15:F16"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="C12:F12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>